<commit_message>
changement au cdc et user stories
</commit_message>
<xml_diff>
--- a/Documents/2020-2021_2T_Document-Coaching-1_Analyse-User-Stories – Copie.xlsx
+++ b/Documents/2020-2021_2T_Document-Coaching-1_Analyse-User-Stories – Copie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23802"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ephec-my.sharepoint.com/personal/he201896_students_ephec_be/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ephec-my.sharepoint.com/personal/he201896_students_ephec_be/Documents/2TI/Development informatique/Projet LibelaShop/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{05F4C373-70E2-4FFA-881C-3F7C0B7613C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CA7EADB2-F387-4C25-AFF4-C3CB39BBA4E5}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{05F4C373-70E2-4FFA-881C-3F7C0B7613C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{353C76AA-16AD-45DC-8943-B771451820DE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="936" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" tabRatio="936" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Infos-Coaching" sheetId="47" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="virginie2">#REF!</definedName>
     <definedName name="xavier1">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Rappel bref du fonctionnement des coachings : lecture, préparations, déroulement, rattrapages</t>
   </si>
@@ -113,6 +113,9 @@
     <t>Etudiant responsable de présenter durant ce coaching -ci :</t>
   </si>
   <si>
+    <t>Morgan Holsters</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t>Liens vers la présentation du client et la description des interactions sur le wiki :</t>
   </si>
   <si>
+    <t>https://github.com/MorganHolsters/Projet-LibelaShop/blob/main/Documents/06022021_CDC.docx</t>
+  </si>
+  <si>
     <t>R2</t>
   </si>
   <si>
@@ -225,13 +231,16 @@
   </si>
   <si>
     <t>Commentaires à souligner (notamment améliorations à compléter et dates limites)</t>
+  </si>
+  <si>
+    <t>https://github.com/MorganHolsters/Projet-LibelaShop/wiki/1.-User-story-09-02-2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -808,74 +817,74 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="6"/>
     <col min="2" max="2" width="165.28515625" style="6" customWidth="1"/>
     <col min="3" max="16384" width="11.42578125" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
@@ -890,10 +899,10 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.42578125" style="6"/>
     <col min="4" max="4" width="54.7109375" customWidth="1"/>
@@ -907,7 +916,7 @@
     <col min="12" max="12" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" s="9"/>
       <c r="D1" s="5" t="s">
         <v>13</v>
@@ -921,7 +930,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="9"/>
       <c r="D2" s="6"/>
       <c r="E2" s="2"/>
@@ -929,7 +938,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
@@ -943,7 +952,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
       <c r="D4" s="7" t="s">
         <v>16</v>
@@ -953,7 +962,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
@@ -964,7 +973,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="6"/>
       <c r="D7" s="7" t="s">
         <v>18</v>
@@ -976,7 +985,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -986,7 +995,7 @@
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
@@ -997,133 +1006,139 @@
       <c r="G9" s="26"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="12"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="19"/>
       <c r="G10" s="20"/>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="19"/>
       <c r="G11" s="20"/>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="6"/>
       <c r="D12" s="30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="19"/>
       <c r="G12" s="20"/>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="19"/>
       <c r="G13" s="20"/>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="6"/>
-      <c r="D14" s="10"/>
+      <c r="D14" s="30" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="19"/>
       <c r="G14" s="20"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="19"/>
       <c r="G15" s="20"/>
       <c r="H15" s="21"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="12"/>
       <c r="C16" s="6"/>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="19"/>
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="19"/>
       <c r="G17" s="20"/>
       <c r="H17" s="21"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="12"/>
       <c r="C18" s="6"/>
       <c r="D18" s="30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="19"/>
       <c r="G18" s="20"/>
       <c r="H18" s="21"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="22"/>
       <c r="G19" s="23"/>
       <c r="H19" s="24"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" s="6"/>
       <c r="D20" s="30" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="7"/>
@@ -1132,29 +1147,29 @@
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="1:8" s="6" customFormat="1">
+    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="9"/>
       <c r="C23" s="18"/>
       <c r="D23" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:8" s="6" customFormat="1">
+    <row r="24" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1162,191 +1177,191 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="1:8" s="6" customFormat="1">
+    <row r="26" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:8" s="6" customFormat="1">
+    <row r="27" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" s="6" customFormat="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" s="6" customFormat="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="6" customFormat="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:4" s="6" customFormat="1">
+    <row r="43" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="6" customFormat="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C49" s="9"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C50" s="6"/>
       <c r="D50" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1354,12 +1369,22 @@
     <hyperlink ref="D20" r:id="rId1" xr:uid="{297364F0-2A9B-4BDB-A30E-EA597A69B5D1}"/>
     <hyperlink ref="D18" r:id="rId2" xr:uid="{171CD3B9-E02E-4D1C-AF52-0AFD76A9D012}"/>
     <hyperlink ref="D12" r:id="rId3" location="projet-libelashop" xr:uid="{021FD8CA-765B-4D74-A759-C5F250158C03}"/>
+    <hyperlink ref="D14" r:id="rId4" xr:uid="{33E35456-90C6-4C36-86BF-3890AF00B113}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008E426C959392C4495866AB4282E88A2" ma:contentTypeVersion="4" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="88602fbb6dfee49a9b9a642df555fbe3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2a71c00b-36d5-4019-8799-c95aa119f5e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="376f1a1869678f9d943b1e9fcf55f3d8" ns2:_="">
     <xsd:import namespace="2a71c00b-36d5-4019-8799-c95aa119f5e6"/>
@@ -1505,29 +1530,43 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7031F772-C6CD-4B1D-898D-6EE31E9FCE99}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBE24235-C4C2-411B-BE20-DD532525DB51}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2326994-45D9-4231-8DA3-DF51167BC379}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7031F772-C6CD-4B1D-898D-6EE31E9FCE99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2a71c00b-36d5-4019-8799-c95aa119f5e6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBE24235-C4C2-411B-BE20-DD532525DB51}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2326994-45D9-4231-8DA3-DF51167BC379}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>